<commit_message>
fixed a bug in the year calculation of immig/pop
</commit_message>
<xml_diff>
--- a/data/app_flyktninger_oppsummert.xlsx
+++ b/data/app_flyktninger_oppsummert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://llano279-my.sharepoint.com/personal/oivind_lla_no/Documents/Prosjekter/p04-ukraina/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_107C7EC18F79A8D366075C52F37BD2720A5AA628" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D41D1E5-38F6-5449-A421-4FE8CDA09C65}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_107C7EC18F79A8D366075C52F37BD2720A5AA628" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFF129F3-CFA8-9B47-968F-A49450CF9344}"/>
   <bookViews>
-    <workbookView xWindow="-15560" yWindow="-19500" windowWidth="32220" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="7100" windowWidth="17840" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4495,7 +4495,7 @@
   <dimension ref="A1:AL1072"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P127" sqref="P127:P841"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14952,7 +14952,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="127" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>2022</v>
       </c>
@@ -31089,7 +31089,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="322" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>2022</v>
       </c>
@@ -32556,7 +32556,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="340" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>2022</v>
       </c>
@@ -44397,7 +44397,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="484" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A484">
         <v>2023</v>
       </c>
@@ -60543,7 +60543,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="679" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="679" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A679">
         <v>2023</v>
       </c>
@@ -62019,7 +62019,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="697" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="697" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A697">
         <v>2023</v>
       </c>
@@ -76401,7 +76401,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="841" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="841" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A841">
         <v>2024</v>
       </c>
@@ -96183,7 +96183,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="1036" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1036" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1036">
         <v>2024</v>
       </c>
@@ -97956,7 +97956,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="1054" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1054" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A1054">
         <v>2024</v>
       </c>
@@ -99825,7 +99825,8 @@
   <autoFilter ref="A1:AL1072" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Drammen"/>
+        <filter val="Kvæfjord"/>
+        <filter val="Kvænangen"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>